<commit_message>
update with flight logs
</commit_message>
<xml_diff>
--- a/ListMateriel.xlsx
+++ b/ListMateriel.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2E35E6-A3F0-48DF-BFD3-39F9A927BE84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -129,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,38 +483,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D2">
         <f>SUM(D5:D12)</f>
         <v>239.69</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -536,12 +543,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -568,7 +575,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -598,7 +605,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -628,7 +635,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -658,7 +665,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -688,7 +695,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -718,7 +725,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -748,7 +755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>

</xml_diff>